<commit_message>
Datos y r validación
</commit_message>
<xml_diff>
--- a/AnalisisDeEntrada/Validación.xlsx
+++ b/AnalisisDeEntrada/Validación.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibianagambas/Documents/Universidad de Los Andes/Octavo Semestre/Simulación de Eventos Discretos/Proyecto/SimulationProject/AnalisisDeEntrada/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlospenaloza/Universidad/Simulación/SimulationProject/AnalisisDeEntrada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B364FBF-EF42-2A4E-A636-AF95FF32524B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CFF4F9-FABC-F94C-8DA1-18AA3E5C0C9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validación" sheetId="1" r:id="rId1"/>
     <sheet name="V" sheetId="2" r:id="rId2"/>
     <sheet name="VF" sheetId="3" r:id="rId3"/>
+    <sheet name="DatosValidacion" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Brayan López</t>
   </si>
@@ -105,14 +106,33 @@
   </si>
   <si>
     <t>Juan Jaimes</t>
+  </si>
+  <si>
+    <t>datosP1</t>
+  </si>
+  <si>
+    <t>datosP2</t>
+  </si>
+  <si>
+    <t>datosP3</t>
+  </si>
+  <si>
+    <t>datosP4</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>DesvEst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -166,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,6 +213,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -562,14 +589,14 @@
         <v>0.40625</v>
       </c>
       <c r="E2" s="4">
-        <f>(D2-C2)*24</f>
+        <f t="shared" ref="E2:E11" si="0">(D2-C2)*24</f>
         <v>0.56805555555555598</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*60</f>
+        <f t="shared" ref="F2:F11" si="1">E2*60</f>
         <v>34.083333333333357</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="12">
         <f>AVERAGE(F2:F4)</f>
         <v>31.616666666666649</v>
       </c>
@@ -592,14 +619,14 @@
         <v>0.54027777777777775</v>
       </c>
       <c r="E3" s="4">
-        <f>(D3-C3)*24</f>
+        <f t="shared" si="0"/>
         <v>0.32722222222222097</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*60</f>
+        <f t="shared" si="1"/>
         <v>19.633333333333258</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -615,14 +642,14 @@
         <v>0.42569444444444443</v>
       </c>
       <c r="E4" s="4">
-        <f>(D4-C4)*24</f>
+        <f t="shared" si="0"/>
         <v>0.6855555555555557</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*60</f>
+        <f t="shared" si="1"/>
         <v>41.13333333333334</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -638,14 +665,14 @@
         <v>0.43333333333333335</v>
       </c>
       <c r="E5" s="4">
-        <f>(D5-C5)*24</f>
+        <f t="shared" si="0"/>
         <v>0.75138888888888999</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*60</f>
+        <f t="shared" si="1"/>
         <v>45.0833333333334</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="12">
         <f>AVERAGE(F5:F9)</f>
         <v>68.660000000000053</v>
       </c>
@@ -668,14 +695,14 @@
         <v>0.66805555555555562</v>
       </c>
       <c r="E6" s="4">
-        <f>(D6-C6)*24</f>
+        <f t="shared" si="0"/>
         <v>0.81166666666666831</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*60</f>
+        <f t="shared" si="1"/>
         <v>48.700000000000102</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -691,14 +718,14 @@
         <v>0.41388888888888892</v>
       </c>
       <c r="E7" s="4">
-        <f>(D7-C7)*24</f>
+        <f t="shared" si="0"/>
         <v>2.1572222222222219</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*60</f>
+        <f t="shared" si="1"/>
         <v>129.43333333333331</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -714,14 +741,14 @@
         <v>0.46875</v>
       </c>
       <c r="E8" s="4">
-        <f>(D8-C8)*24</f>
+        <f t="shared" si="0"/>
         <v>0.72111111111111237</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*60</f>
+        <f t="shared" si="1"/>
         <v>43.266666666666744</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -737,14 +764,14 @@
         <v>0.40208333333333335</v>
       </c>
       <c r="E9" s="4">
-        <f>(D9-C9)*24</f>
+        <f t="shared" si="0"/>
         <v>1.2802777777777785</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*60</f>
+        <f t="shared" si="1"/>
         <v>76.816666666666706</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -760,11 +787,11 @@
         <v>0.49444444444444446</v>
       </c>
       <c r="E10" s="4">
-        <f>(D10-C10)*24</f>
+        <f t="shared" si="0"/>
         <v>1.0144444444444449</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*60</f>
+        <f t="shared" si="1"/>
         <v>60.866666666666696</v>
       </c>
       <c r="G10" s="1">
@@ -786,11 +813,11 @@
         <v>0.36805555555555558</v>
       </c>
       <c r="E11" s="4">
-        <f>(D11-C11)*24</f>
+        <f t="shared" si="0"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*60</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="G11" s="1">
@@ -809,11 +836,11 @@
         <v>0.4152777777777778</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" ref="E12:E21" si="0">(D12-C12)*24</f>
+        <f t="shared" ref="E12:E21" si="2">(D12-C12)*24</f>
         <v>1.0041666666666664</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" ref="F12:F21" si="1">E12*60</f>
+        <f t="shared" ref="F12:F21" si="3">E12*60</f>
         <v>60.249999999999986</v>
       </c>
     </row>
@@ -828,11 +855,11 @@
         <v>0.46875</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.72111111111111237</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43.266666666666744</v>
       </c>
     </row>
@@ -847,11 +874,11 @@
         <v>0.40208333333333335</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2802777777777785</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>76.816666666666706</v>
       </c>
     </row>
@@ -866,11 +893,11 @@
         <v>0.49444444444444446</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0144444444444449</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>60.866666666666696</v>
       </c>
     </row>
@@ -885,11 +912,11 @@
         <v>0.36805555555555558</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
     </row>
@@ -904,11 +931,11 @@
         <v>0.40625</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.56805555555555598</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34.083333333333357</v>
       </c>
     </row>
@@ -923,11 +950,11 @@
         <v>0.54027777777777775</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.32722222222222097</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>19.633333333333258</v>
       </c>
     </row>
@@ -942,11 +969,11 @@
         <v>0.42569444444444443</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6855555555555557</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41.13333333333334</v>
       </c>
     </row>
@@ -961,11 +988,11 @@
         <v>0.43333333333333335</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.75138888888888999</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45.0833333333334</v>
       </c>
     </row>
@@ -980,11 +1007,11 @@
         <v>0.66805555555555562</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.81166666666666831</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>48.700000000000102</v>
       </c>
     </row>
@@ -1005,7 +1032,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1055,14 +1082,14 @@
         <v>0.40625</v>
       </c>
       <c r="E2" s="4">
-        <f>(D2-C2)*24</f>
+        <f t="shared" ref="E2:E10" si="0">(D2-C2)*24</f>
         <v>0.56805555555555598</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*60</f>
+        <f t="shared" ref="F2:F10" si="1">E2*60</f>
         <v>34.083333333333357</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="12">
         <f>AVERAGE(F2:F4)</f>
         <v>31.616666666666649</v>
       </c>
@@ -1085,14 +1112,14 @@
         <v>0.54027777777777775</v>
       </c>
       <c r="E3" s="4">
-        <f>(D3-C3)*24</f>
+        <f t="shared" si="0"/>
         <v>0.32722222222222097</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*60</f>
+        <f t="shared" si="1"/>
         <v>19.633333333333258</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1108,14 +1135,14 @@
         <v>0.42569444444444443</v>
       </c>
       <c r="E4" s="4">
-        <f>(D4-C4)*24</f>
+        <f t="shared" si="0"/>
         <v>0.6855555555555557</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*60</f>
+        <f t="shared" si="1"/>
         <v>41.13333333333334</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1131,14 +1158,14 @@
         <v>0.43333333333333335</v>
       </c>
       <c r="E5" s="4">
-        <f>(D5-C5)*24</f>
+        <f t="shared" si="0"/>
         <v>0.75138888888888999</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*60</f>
+        <f t="shared" si="1"/>
         <v>45.0833333333334</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="12">
         <f>AVERAGE(F5:F9)</f>
         <v>68.660000000000053</v>
       </c>
@@ -1161,14 +1188,14 @@
         <v>0.66805555555555562</v>
       </c>
       <c r="E6" s="4">
-        <f>(D6-C6)*24</f>
+        <f t="shared" si="0"/>
         <v>0.81166666666666831</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*60</f>
+        <f t="shared" si="1"/>
         <v>48.700000000000102</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1184,14 +1211,14 @@
         <v>0.41388888888888892</v>
       </c>
       <c r="E7" s="4">
-        <f>(D7-C7)*24</f>
+        <f t="shared" si="0"/>
         <v>2.1572222222222219</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*60</f>
+        <f t="shared" si="1"/>
         <v>129.43333333333331</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -1207,14 +1234,14 @@
         <v>0.46875</v>
       </c>
       <c r="E8" s="4">
-        <f>(D8-C8)*24</f>
+        <f t="shared" si="0"/>
         <v>0.72111111111111237</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*60</f>
+        <f t="shared" si="1"/>
         <v>43.266666666666744</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1230,14 +1257,14 @@
         <v>0.40208333333333335</v>
       </c>
       <c r="E9" s="4">
-        <f>(D9-C9)*24</f>
+        <f t="shared" si="0"/>
         <v>1.2802777777777785</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*60</f>
+        <f t="shared" si="1"/>
         <v>76.816666666666706</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1253,14 +1280,14 @@
         <v>0.49444444444444446</v>
       </c>
       <c r="E10" s="4">
-        <f>(D10-C10)*24</f>
+        <f t="shared" si="0"/>
         <v>1.0144444444444449</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*60</f>
+        <f t="shared" si="1"/>
         <v>60.866666666666696</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="12">
         <f>AVERAGE(F10:F11)</f>
         <v>82.983333333333334</v>
       </c>
@@ -1283,14 +1310,14 @@
         <v>0.57152777777777775</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:E13" si="0">(D11-C11)*24</f>
+        <f t="shared" ref="E11:E13" si="2">(D11-C11)*24</f>
         <v>1.751666666666666</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F13" si="1">E11*60</f>
+        <f t="shared" ref="F11:F13" si="3">E11*60</f>
         <v>105.09999999999997</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1306,14 +1333,14 @@
         <v>0.36805555555555558</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="12">
         <f>AVERAGE(F12:F13)</f>
         <v>88.658333333333331</v>
       </c>
@@ -1336,14 +1363,14 @@
         <v>0.50069444444444444</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.805277777777778</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>108.31666666666668</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1471,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65169429-ADB8-8D4C-B247-FA7FEA26BDF7}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1495,42 +1522,369 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <f>V!G2</f>
-        <v>31.616666666666649</v>
-      </c>
-      <c r="C2">
-        <f>V!G5</f>
-        <v>68.660000000000053</v>
-      </c>
-      <c r="D2">
-        <f>V!G10</f>
-        <v>82.983333333333334</v>
-      </c>
-      <c r="E2">
-        <f>V!G12</f>
-        <v>88.658333333333331</v>
+      <c r="B2" s="10">
+        <f>DatosValidacion!B17</f>
+        <v>34.562000000000005</v>
+      </c>
+      <c r="C2" s="10">
+        <f>DatosValidacion!C17</f>
+        <v>54.446666666666665</v>
+      </c>
+      <c r="D2" s="10">
+        <f>DatosValidacion!D17</f>
+        <v>83.927333333333323</v>
+      </c>
+      <c r="E2" s="10">
+        <f>DatosValidacion!E17</f>
+        <v>98.977333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3">
-        <f>V!H2</f>
-        <v>10.960193124819217</v>
-      </c>
-      <c r="C3">
-        <f>V!H5</f>
-        <v>36.602634619807183</v>
-      </c>
-      <c r="D3">
-        <f>V!H10</f>
-        <v>31.277689954484874</v>
-      </c>
-      <c r="E3">
-        <f>V!H12</f>
-        <v>27.801081613651146</v>
+      <c r="B3" s="10">
+        <f>DatosValidacion!B18</f>
+        <v>11.112836978660543</v>
+      </c>
+      <c r="C3" s="10">
+        <f>DatosValidacion!C18</f>
+        <v>13.11245790769043</v>
+      </c>
+      <c r="D3" s="10">
+        <f>DatosValidacion!D18</f>
+        <v>19.581114978711657</v>
+      </c>
+      <c r="E3" s="10">
+        <f>DatosValidacion!E18</f>
+        <v>16.11461602160627</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F493F51-829E-E84C-ACCA-92467829DA6D}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>46.46</v>
+      </c>
+      <c r="C2" s="5">
+        <v>34.74</v>
+      </c>
+      <c r="D2" s="5">
+        <v>90.69</v>
+      </c>
+      <c r="E2" s="5">
+        <v>89.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>32.29</v>
+      </c>
+      <c r="C3" s="5">
+        <v>46.71</v>
+      </c>
+      <c r="D3" s="5">
+        <v>73.38</v>
+      </c>
+      <c r="E3" s="5">
+        <v>80.69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>22.63</v>
+      </c>
+      <c r="C4" s="5">
+        <v>47.86</v>
+      </c>
+      <c r="D4" s="5">
+        <v>76.540000000000006</v>
+      </c>
+      <c r="E4" s="5">
+        <v>78.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>41.29</v>
+      </c>
+      <c r="C5" s="5">
+        <v>65.28</v>
+      </c>
+      <c r="D5" s="5">
+        <v>78.06</v>
+      </c>
+      <c r="E5" s="5">
+        <v>77.72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>21.82</v>
+      </c>
+      <c r="C6" s="5">
+        <v>74.349999999999994</v>
+      </c>
+      <c r="D6" s="5">
+        <v>101.97</v>
+      </c>
+      <c r="E6" s="5">
+        <v>81.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>28.22</v>
+      </c>
+      <c r="C7" s="5">
+        <v>39.979999999999997</v>
+      </c>
+      <c r="D7" s="5">
+        <v>99.68</v>
+      </c>
+      <c r="E7" s="5">
+        <v>111.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>36.6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>68.069999999999993</v>
+      </c>
+      <c r="D8" s="5">
+        <v>105.26</v>
+      </c>
+      <c r="E8" s="5">
+        <v>113.53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="C9" s="5">
+        <v>60.07</v>
+      </c>
+      <c r="D9" s="5">
+        <v>84.5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>106.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>47.09</v>
+      </c>
+      <c r="C10" s="5">
+        <v>34.58</v>
+      </c>
+      <c r="D10" s="5">
+        <v>74.28</v>
+      </c>
+      <c r="E10" s="5">
+        <v>112.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>19.55</v>
+      </c>
+      <c r="C11" s="5">
+        <v>60.37</v>
+      </c>
+      <c r="D11" s="5">
+        <v>40.15</v>
+      </c>
+      <c r="E11" s="5">
+        <v>86.72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>49.13</v>
+      </c>
+      <c r="C12" s="5">
+        <v>62.65</v>
+      </c>
+      <c r="D12" s="5">
+        <v>53.75</v>
+      </c>
+      <c r="E12" s="5">
+        <v>115.51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>35.49</v>
+      </c>
+      <c r="C13" s="5">
+        <v>68.260000000000005</v>
+      </c>
+      <c r="D13" s="5">
+        <v>103.09</v>
+      </c>
+      <c r="E13" s="5">
+        <v>117.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>54.68</v>
+      </c>
+      <c r="C14" s="5">
+        <v>41.48</v>
+      </c>
+      <c r="D14" s="5">
+        <v>72.8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>94.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>24.55</v>
+      </c>
+      <c r="C15" s="5">
+        <v>63.69</v>
+      </c>
+      <c r="D15" s="5">
+        <v>101.84</v>
+      </c>
+      <c r="E15" s="5">
+        <v>123.71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>25.29</v>
+      </c>
+      <c r="C16" s="5">
+        <v>48.61</v>
+      </c>
+      <c r="D16" s="5">
+        <v>102.92</v>
+      </c>
+      <c r="E16" s="5">
+        <v>93.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11">
+        <f>AVERAGE(B2:B16)</f>
+        <v>34.562000000000005</v>
+      </c>
+      <c r="C17" s="11">
+        <f>AVERAGE(C2:C16)</f>
+        <v>54.446666666666665</v>
+      </c>
+      <c r="D17" s="11">
+        <f>AVERAGE(D2:D16)</f>
+        <v>83.927333333333323</v>
+      </c>
+      <c r="E17" s="11">
+        <f>AVERAGE(E2:E16)</f>
+        <v>98.977333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="11">
+        <f>STDEV(B2:B16)</f>
+        <v>11.112836978660543</v>
+      </c>
+      <c r="C18" s="11">
+        <f>STDEV(C2:C16)</f>
+        <v>13.11245790769043</v>
+      </c>
+      <c r="D18" s="11">
+        <f>STDEV(D2:D16)</f>
+        <v>19.581114978711657</v>
+      </c>
+      <c r="E18" s="11">
+        <f>STDEV(E2:E16)</f>
+        <v>16.11461602160627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>